<commit_message>
changed plan and cases
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3190" yWindow="4740" windowWidth="22960" windowHeight="10400"/>
+    <workbookView xWindow="2060" yWindow="4410" windowWidth="22960" windowHeight="10400"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="277">
   <si>
     <t>Группа проверок</t>
   </si>
@@ -755,13 +755,261 @@
 2. Открываются настройки
 3. Включается темная тема, экран становится черным, а текст белым
 4. Текстовая область в новостях и цитатах сновится частично темной, а текст белым. Если фон до этого был другого цвета (в цитатах и в новостях в плашке дата), то текст там не читается</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Создаие новости с редактированием поля "категория"</t>
+  </si>
+  <si>
+    <t>1. Нажать на кнопку редактирования новости
+2. Корректно заполнить все поля (выбрать категорию, запланировать дату и время публикации, указать заголовок и содержание новости)
+3. Нажать на поле "категория", ввести любые знаки (например, цифры "123")
+4. Нажать сохранить
+5. Новость не сохраняется, появляется сообщение об ошибке</t>
+  </si>
+  <si>
+    <t>Редактирование новости</t>
+  </si>
+  <si>
+    <t>1. Нажать на кнопку редактирования новости
+2. Внести любые изменения, например в содержание
+3. Нажать на кнопку "сохранить"
+4. Содержание, категория, заголовок, дата публикации соотвествуют заданным, дата создания соотвествует текущему времени</t>
+  </si>
+  <si>
+    <t>1. Открывается окно редактирования новости
+2. Отображаются внесенные изменения
+3. Новость сохраняется со статусом "активна"
+4. Данные новости соотвествуют заполненным данным, дата создания соответствует текущей дате</t>
+  </si>
+  <si>
+    <t>1. Открывается окно редактирования новости
+2. Отображаются внесенные изменения
+3. Новость сохраняется со статусом "активна"
+4. Данные новости соотвествуют заполненным данным, дата создания отображается некорректно</t>
+  </si>
+  <si>
+    <t>Создание более 8 активных новостей</t>
+  </si>
+  <si>
+    <t>1. Создать 8 аквтиных новостей
+2. Создать и сохранить новую новость с корректным заполнением новостей
+3. Проверить количество новостей</t>
+  </si>
+  <si>
+    <t>1. Отображается 8 активных новостей
+2. Новость успешно сохраняется
+3. На странице новостей 9 активных новостей</t>
+  </si>
+  <si>
+    <t>1. Отображается 8 активных новостей
+2. Новость успешно сохраняется
+3. На странице новостей все еще 8 активных новостей, самая ранняя исчезла
+(Т.к. нет документации, может быть не багом, а фичей)</t>
+  </si>
+  <si>
+    <t>AUTH_visible</t>
+  </si>
+  <si>
+    <t>AUTH_login_success</t>
+  </si>
+  <si>
+    <t>AUTH_login_fail</t>
+  </si>
+  <si>
+    <t>AUTH_empty</t>
+  </si>
+  <si>
+    <t>AUTH_emptylog</t>
+  </si>
+  <si>
+    <t>AUTH_emptypass</t>
+  </si>
+  <si>
+    <t>AUTH_validsymbols</t>
+  </si>
+  <si>
+    <t>AUTH_invalidlog</t>
+  </si>
+  <si>
+    <t>AUTH_invalidpass</t>
+  </si>
+  <si>
+    <t>AUTH_sql_log</t>
+  </si>
+  <si>
+    <t>AUTH_xss_log</t>
+  </si>
+  <si>
+    <t>AUTH_sql_pass</t>
+  </si>
+  <si>
+    <t>AUTH_xss_pass</t>
+  </si>
+  <si>
+    <t>MAIN_visible</t>
+  </si>
+  <si>
+    <t>MAIN_expand_news</t>
+  </si>
+  <si>
+    <t>MAIN_upd</t>
+  </si>
+  <si>
+    <t>MAIN_allnews</t>
+  </si>
+  <si>
+    <t>MAIN_expand_newsblock</t>
+  </si>
+  <si>
+    <t>NAV_quotes</t>
+  </si>
+  <si>
+    <t>NAV_logout</t>
+  </si>
+  <si>
+    <t>NAV_menu_mainpage</t>
+  </si>
+  <si>
+    <t>NAV_menu_anotherpage</t>
+  </si>
+  <si>
+    <t>NAV_about_mainpage</t>
+  </si>
+  <si>
+    <t>NAV_about_news</t>
+  </si>
+  <si>
+    <t>NAV_about_quotes</t>
+  </si>
+  <si>
+    <t>NAV_about_return</t>
+  </si>
+  <si>
+    <t>NEWS_visible</t>
+  </si>
+  <si>
+    <t>NEWS_expand</t>
+  </si>
+  <si>
+    <t>NEWS_upd</t>
+  </si>
+  <si>
+    <t>NEWS_scroll</t>
+  </si>
+  <si>
+    <t>NEWS_sort</t>
+  </si>
+  <si>
+    <t>NEWS_open_filter</t>
+  </si>
+  <si>
+    <t>NEWS_filter_by_date</t>
+  </si>
+  <si>
+    <t>NEWS_filter_by_category</t>
+  </si>
+  <si>
+    <t>NEWS_filter_cancel</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_scroll</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_sort</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_deletenews</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_canceldelete</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_canceledit</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_editnews</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_createnews</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_create_editcategory</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_create_fill_russian</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_create_more8news</t>
+  </si>
+  <si>
+    <t>NEWSCONTROL_create_with_empty_space</t>
+  </si>
+  <si>
+    <t>QUOTES_visible</t>
+  </si>
+  <si>
+    <t>QUOTES_expand</t>
+  </si>
+  <si>
+    <t>QUOTES_scroll</t>
+  </si>
+  <si>
+    <t>ABOUT_visible</t>
+  </si>
+  <si>
+    <t>ABOUT_pp</t>
+  </si>
+  <si>
+    <t>ABOUT_tou</t>
+  </si>
+  <si>
+    <t>NET_wifi</t>
+  </si>
+  <si>
+    <t>NET_mobile</t>
+  </si>
+  <si>
+    <t>NET_withoutsignal</t>
+  </si>
+  <si>
+    <t>NET_flightmode</t>
+  </si>
+  <si>
+    <t>UI_landscape</t>
+  </si>
+  <si>
+    <t>UI_call</t>
+  </si>
+  <si>
+    <t>UI_message</t>
+  </si>
+  <si>
+    <t>UI_volume</t>
+  </si>
+  <si>
+    <t>UI_collapseapp</t>
+  </si>
+  <si>
+    <t>UI_expandapp</t>
+  </si>
+  <si>
+    <t>UI_return</t>
+  </si>
+  <si>
+    <t>UI_darkmoode</t>
+  </si>
+  <si>
+    <t>авт</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -786,6 +1034,13 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -801,7 +1056,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -836,7 +1091,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -857,21 +1112,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -890,21 +1130,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -914,25 +1139,8 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -942,7 +1150,35 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -953,20 +1189,120 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -976,30 +1312,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1008,43 +1335,79 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1341,1354 +1704,1695 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62:G62"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="67.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6328125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="24.7265625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="37.81640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="35.54296875" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="24" style="10" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="24.7265625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="37.81640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="35.54296875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="36"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" thickBot="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="28.5" thickBot="1">
+      <c r="A1" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="56">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:9" ht="56">
+      <c r="A2" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="F2" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="15" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="140">
-      <c r="A3" s="6"/>
-      <c r="B3" s="11" t="s">
+      <c r="I2" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="140">
+      <c r="A3" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="15" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="126">
-      <c r="A4" s="6"/>
-      <c r="B4" s="11" t="s">
+      <c r="I3" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="126">
+      <c r="A4" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="G4" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="15" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="98">
-      <c r="A5" s="6"/>
-      <c r="B5" s="11" t="s">
+      <c r="I4" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="98">
+      <c r="A5" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="15" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="112">
-      <c r="A6" s="6"/>
-      <c r="B6" s="11" t="s">
+      <c r="I5" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="112">
+      <c r="A6" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="G6" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="112">
-      <c r="A7" s="6"/>
-      <c r="B7" s="11" t="s">
+    <row r="7" spans="1:9" ht="112">
+      <c r="A7" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="H7" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="126">
-      <c r="A8" s="6"/>
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:9" ht="126">
+      <c r="A8" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="F8" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="G8" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="H8" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="84">
-      <c r="A9" s="6"/>
-      <c r="B9" s="23" t="s">
+    <row r="9" spans="1:9" ht="84">
+      <c r="A9" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="D9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="E9" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="F9" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="G9" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="84">
-      <c r="A10" s="6"/>
-      <c r="B10" s="23" t="s">
+    <row r="10" spans="1:9" ht="84">
+      <c r="A10" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="D10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="E10" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="F10" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="G10" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="H10" s="21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="140">
-      <c r="A11" s="6"/>
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="1:9" ht="140">
+      <c r="A11" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="F11" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="G11" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="H11" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="140">
-      <c r="A12" s="15"/>
-      <c r="B12" s="11" t="s">
+    <row r="12" spans="1:9" ht="140">
+      <c r="A12" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="F12" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="G12" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="H12" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="140.5" thickBot="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="1:9" ht="140">
+      <c r="A13" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="F13" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="G13" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="H13" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="155" customHeight="1" thickBot="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="12" t="s">
+    <row r="14" spans="1:9" ht="155" customHeight="1" thickBot="1">
+      <c r="A14" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="F14" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="G14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="H14" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="168">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:9" ht="168">
+      <c r="A15" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="F15" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="G15" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="H15" s="15" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="84">
-      <c r="A16" s="6"/>
-      <c r="B16" s="11" t="s">
+      <c r="I15" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="84">
+      <c r="A16" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="F16" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="G16" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="H16" s="15" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="98">
-      <c r="A17" s="6"/>
-      <c r="B17" s="11" t="s">
+      <c r="I16" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="98">
+      <c r="A17" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="E17" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="F17" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="G17" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="H17" s="15" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="56">
-      <c r="A18" s="6"/>
-      <c r="B18" s="20" t="s">
+      <c r="I17" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="56">
+      <c r="A18" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="D18" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="E18" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="F18" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="G18" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="H18" s="18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.5" thickBot="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="12" t="s">
+    <row r="19" spans="1:9" ht="28.5" thickBot="1">
+      <c r="A19" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="F19" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="G19" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="H19" s="15" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="42">
-      <c r="A20" s="4" t="s">
+      <c r="I19" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="42">
+      <c r="A20" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B20" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="F20" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="G20" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="H20" s="15" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="56">
-      <c r="A21" s="6"/>
-      <c r="B21" s="11" t="s">
+      <c r="I20" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="56">
+      <c r="A21" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="F21" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="G21" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="H21" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="42">
-      <c r="A22" s="6"/>
-      <c r="B22" s="11" t="s">
+      <c r="I21" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="42">
+      <c r="A22" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="F22" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="G22" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="H22" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="42">
-      <c r="A23" s="6"/>
-      <c r="B23" s="11" t="s">
+    <row r="23" spans="1:9" ht="42">
+      <c r="A23" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="F23" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="G23" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="H23" s="15" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="98">
-      <c r="A24" s="6"/>
-      <c r="B24" s="11" t="s">
+    <row r="24" spans="1:9" ht="98">
+      <c r="A24" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="F24" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="G24" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="H24" s="15" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="98">
-      <c r="A25" s="6"/>
-      <c r="B25" s="20" t="s">
+      <c r="I24" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="98">
+      <c r="A25" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="D25" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="E25" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="F25" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="G25" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="H25" s="18" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="98">
-      <c r="A26" s="6"/>
-      <c r="B26" s="11" t="s">
+      <c r="I25" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="98">
+      <c r="A26" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="F26" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="19" t="s">
+      <c r="G26" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="H26" s="15" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="112.5" thickBot="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="12" t="s">
+    <row r="27" spans="1:9" ht="112.5" thickBot="1">
+      <c r="A27" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="E27" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="F27" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="G27" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="H27" s="15" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="140">
-      <c r="A28" s="4" t="s">
+      <c r="I27" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="140">
+      <c r="A28" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B28" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="C28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="F28" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="G28" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="H28" s="15" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="98">
-      <c r="A29" s="6"/>
-      <c r="B29" s="11" t="s">
+      <c r="I28" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="98">
+      <c r="A29" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="F29" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="G29" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="H29" s="15" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="56">
-      <c r="A30" s="6"/>
-      <c r="B30" s="11" t="s">
+      <c r="I29" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="56">
+      <c r="A30" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="E30" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="F30" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="G30" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="H30" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="70">
-      <c r="A31" s="6"/>
-      <c r="B31" s="11" t="s">
+    <row r="31" spans="1:9" ht="70">
+      <c r="A31" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="E31" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="F31" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="G31" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="H31" s="15" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="42">
-      <c r="A32" s="6"/>
-      <c r="B32" s="11" t="s">
+    <row r="32" spans="1:9" ht="42">
+      <c r="A32" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="F32" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="F32" s="19" t="s">
+      <c r="G32" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="H32" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="42">
-      <c r="A33" s="6"/>
-      <c r="B33" s="11" t="s">
+    <row r="33" spans="1:9" ht="42">
+      <c r="A33" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="F33" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="G33" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="H33" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="140">
-      <c r="A34" s="6"/>
-      <c r="B34" s="11" t="s">
+    <row r="34" spans="1:9" ht="140">
+      <c r="A34" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="F34" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="G34" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="H34" s="15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="112">
-      <c r="A35" s="6"/>
-      <c r="B35" s="11" t="s">
+    <row r="35" spans="1:9" ht="112">
+      <c r="A35" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="F35" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="G35" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="H35" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="112">
-      <c r="A36" s="6"/>
-      <c r="B36" s="11" t="s">
+    <row r="36" spans="1:9" ht="112">
+      <c r="A36" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="E36" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="F36" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="G36" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="H36" s="15" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="98">
-      <c r="A37" s="6"/>
-      <c r="B37" s="11" t="s">
+      <c r="I36" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="98">
+      <c r="A37" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="E37" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="F37" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="G37" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="H37" s="15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="112">
-      <c r="A38" s="6"/>
-      <c r="B38" s="11" t="s">
+    <row r="38" spans="1:9" ht="112">
+      <c r="A38" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="F38" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="G38" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="H38" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="84">
-      <c r="A39" s="6"/>
-      <c r="B39" s="11" t="s">
+    <row r="39" spans="1:9" ht="84">
+      <c r="A39" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="F39" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="F39" s="19" t="s">
+      <c r="G39" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="H39" s="15" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="84">
-      <c r="A40" s="6"/>
-      <c r="B40" s="11" t="s">
+      <c r="I39" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="84">
+      <c r="A40" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="F40" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="G40" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="H40" s="15" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="154">
-      <c r="A41" s="6"/>
-      <c r="B41" s="11" t="s">
+      <c r="I40" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="154">
+      <c r="A41" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="D41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="E41" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="F41" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="G41" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="H41" s="15" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="210">
-      <c r="A42" s="6"/>
-      <c r="B42" s="20" t="s">
+      <c r="I41" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="175.5" customHeight="1">
+      <c r="A42" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B42" s="27"/>
+      <c r="C42" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="I42" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="210">
+      <c r="A43" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B43" s="27"/>
+      <c r="C43" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="20" t="s">
+      <c r="D43" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="F43" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="F42" s="22" t="s">
+      <c r="G43" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G42" s="22" t="s">
+      <c r="H43" s="18" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="238">
-      <c r="A43" s="6"/>
-      <c r="B43" s="20" t="s">
+      <c r="I43" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="233.5" customHeight="1">
+      <c r="A44" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H44" s="21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="238">
+      <c r="A45" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B45" s="27"/>
+      <c r="C45" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="20" t="s">
+      <c r="D45" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="F45" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="F43" s="22" t="s">
+      <c r="G45" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G43" s="22" t="s">
+      <c r="H45" s="18" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="140.5" thickBot="1">
-      <c r="A44" s="8"/>
-      <c r="B44" s="11" t="s">
+    <row r="46" spans="1:9" ht="150" customHeight="1">
+      <c r="A46" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B46" s="28"/>
+      <c r="C46" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="140.5" thickBot="1">
+      <c r="A47" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B47" s="29"/>
+      <c r="C47" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="23" t="s">
+      <c r="D47" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="E44" s="25" t="s">
+      <c r="F47" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="F44" s="25" t="s">
+      <c r="G47" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="G44" s="25" t="s">
+      <c r="H47" s="21" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="56">
-      <c r="A45" s="4" t="s">
+      <c r="I47" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="56">
+      <c r="A48" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B48" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="C48" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="11" t="s">
+      <c r="D48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E45" s="19" t="s">
+      <c r="F48" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="G48" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G45" s="19" t="s">
+      <c r="H48" s="15" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="56">
-      <c r="A46" s="6"/>
-      <c r="B46" s="11" t="s">
+      <c r="I48" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="56">
+      <c r="A49" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B49" s="27"/>
+      <c r="C49" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="11" t="s">
+      <c r="D49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E46" s="19" t="s">
+      <c r="F49" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="G49" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="G46" s="19" t="s">
+      <c r="H49" s="15" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="56.5" thickBot="1">
-      <c r="A47" s="8"/>
-      <c r="B47" s="12" t="s">
+      <c r="I49" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="56.5" thickBot="1">
+      <c r="A50" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B50" s="29"/>
+      <c r="C50" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="D50" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="E50" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E47" s="19" t="s">
+      <c r="F50" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="F47" s="19" t="s">
+      <c r="G50" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="G47" s="19" t="s">
+      <c r="H50" s="15" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="98">
-      <c r="A48" s="4" t="s">
+    <row r="51" spans="1:9" ht="112">
+      <c r="A51" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B51" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="C51" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="11" t="s">
+      <c r="D51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="F51" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="F48" s="19" t="s">
+      <c r="G51" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="G48" s="19" t="s">
+      <c r="H51" s="15" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="56">
-      <c r="A49" s="6"/>
-      <c r="B49" s="20" t="s">
+      <c r="I51" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="56">
+      <c r="A52" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B52" s="27"/>
+      <c r="C52" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="D52" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="20" t="s">
+      <c r="E52" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="E49" s="22" t="s">
+      <c r="F52" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="F49" s="22" t="s">
+      <c r="G52" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="G49" s="22" t="s">
+      <c r="H52" s="18" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="42.5" thickBot="1">
-      <c r="A50" s="8"/>
-      <c r="B50" s="26" t="s">
+      <c r="I52" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="42.5" thickBot="1">
+      <c r="A53" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B53" s="29"/>
+      <c r="C53" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="27" t="s">
+      <c r="D53" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="E53" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="E50" s="22" t="s">
+      <c r="F53" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="F50" s="22" t="s">
+      <c r="G53" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="G50" s="22" t="s">
+      <c r="H53" s="18" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="84">
-      <c r="A51" s="4" t="s">
+      <c r="I53" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="98">
+      <c r="A54" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B54" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="C54" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="11" t="s">
+      <c r="D54" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="F54" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="F51" s="19" t="s">
+      <c r="G54" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="G51" s="19" t="s">
+      <c r="H54" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="84">
-      <c r="A52" s="6"/>
-      <c r="B52" s="11" t="s">
+    <row r="55" spans="1:9" ht="98">
+      <c r="A55" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B55" s="27"/>
+      <c r="C55" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="11" t="s">
+      <c r="D55" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="F55" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="F52" s="19" t="s">
+      <c r="G55" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="G52" s="19" t="s">
+      <c r="H55" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="112">
-      <c r="A53" s="6"/>
-      <c r="B53" s="11" t="s">
+    <row r="56" spans="1:9" ht="112">
+      <c r="A56" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B56" s="27"/>
+      <c r="C56" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="11" t="s">
+      <c r="D56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E53" s="19" t="s">
+      <c r="F56" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="F53" s="19" t="s">
+      <c r="G56" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="G53" s="19" t="s">
+      <c r="H56" s="15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="98.5" thickBot="1">
-      <c r="A54" s="8"/>
-      <c r="B54" s="12" t="s">
+    <row r="57" spans="1:9" ht="98.5" thickBot="1">
+      <c r="A57" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B57" s="29"/>
+      <c r="C57" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="D57" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="E57" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E54" s="19" t="s">
+      <c r="F57" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="F54" s="19" t="s">
+      <c r="G57" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="G54" s="19" t="s">
+      <c r="H57" s="15" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="42">
-      <c r="A55" s="4" t="s">
+    <row r="58" spans="1:9" ht="42">
+      <c r="A58" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B58" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="C58" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="11" t="s">
+      <c r="D58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E55" s="19" t="s">
+      <c r="F58" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="F55" s="19" t="s">
+      <c r="G58" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="G55" s="19" t="s">
+      <c r="H58" s="15" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="42">
-      <c r="A56" s="6"/>
-      <c r="B56" s="11" t="s">
+    <row r="59" spans="1:9" ht="42">
+      <c r="A59" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B59" s="27"/>
+      <c r="C59" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="11" t="s">
+      <c r="D59" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="F59" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="F56" s="19" t="s">
+      <c r="G59" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="G56" s="19" t="s">
+      <c r="H59" s="15" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="42">
-      <c r="A57" s="6"/>
-      <c r="B57" s="11" t="s">
+    <row r="60" spans="1:9" ht="42">
+      <c r="A60" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B60" s="27"/>
+      <c r="C60" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="11" t="s">
+      <c r="D60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="F60" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="G60" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="G57" s="19" t="s">
+      <c r="H60" s="15" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="56">
-      <c r="A58" s="6"/>
-      <c r="B58" s="11" t="s">
+    <row r="61" spans="1:9" ht="56">
+      <c r="A61" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B61" s="27"/>
+      <c r="C61" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="11" t="s">
+      <c r="D61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="F61" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="F58" s="19" t="s">
+      <c r="G61" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="G58" s="19" t="s">
+      <c r="H61" s="15" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="42">
-      <c r="A59" s="6"/>
-      <c r="B59" s="11" t="s">
+    <row r="62" spans="1:9" ht="42">
+      <c r="A62" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B62" s="27"/>
+      <c r="C62" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="11" t="s">
+      <c r="D62" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="F62" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="F59" s="19" t="s">
+      <c r="G62" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="G59" s="19" t="s">
+      <c r="H62" s="15" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="56">
-      <c r="A60" s="6"/>
-      <c r="B60" s="11" t="s">
+    <row r="63" spans="1:9" ht="70">
+      <c r="A63" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B63" s="27"/>
+      <c r="C63" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="11" t="s">
+      <c r="D63" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="19" t="s">
+      <c r="F63" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="F60" s="19" t="s">
+      <c r="G63" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="H63" s="15" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="56">
-      <c r="A61" s="6"/>
-      <c r="B61" s="11" t="s">
+    <row r="64" spans="1:9" ht="56">
+      <c r="A64" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B64" s="27"/>
+      <c r="C64" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="D64" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="E64" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E61" s="19" t="s">
+      <c r="F64" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="F61" s="19" t="s">
+      <c r="G64" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="G61" s="19" t="s">
+      <c r="H64" s="15" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="126.5" thickBot="1">
-      <c r="A62" s="8"/>
-      <c r="B62" s="26" t="s">
+    <row r="65" spans="1:8" ht="140.5" thickBot="1">
+      <c r="A65" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B65" s="29"/>
+      <c r="C65" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="27" t="s">
+      <c r="D65" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="20" t="s">
+      <c r="E65" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E62" s="22" t="s">
+      <c r="F65" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="F62" s="22" t="s">
+      <c r="G65" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="G62" s="22" t="s">
+      <c r="H65" s="18" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A62"/>
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="A28:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B58:B65"/>
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B20:B27"/>
+    <mergeCell ref="B28:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
added allure report and bug-reports
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -551,12 +551,6 @@
 4. Новость остается без изменений</t>
   </si>
   <si>
-    <t>1. Нажать на кнопку редактирования новости
-2. Корректно заполнить все поля (выбрать категорию, запланировать дату и время публикации, указать заголовок и содержание новости)
-3. Нажать сохранить
-4. Содержание, категория, заголовок, дата публикации соотвествуют заданным, дата создания соотвествует текущему времени</t>
-  </si>
-  <si>
     <t>1. Открывается окно редактирования новости
 2. В полях отображаются корректно введенные данные
 3. Новость сохраняется со статусом "активна"
@@ -1003,6 +997,12 @@
   </si>
   <si>
     <t>авт</t>
+  </si>
+  <si>
+    <t>1. Нажать на кнопку создания новости
+2. Корректно заполнить все поля (выбрать категорию, запланировать дату и время публикации, указать заголовок и содержание новости)
+3. Нажать сохранить
+4. Содержание, категория, заголовок, дата публикации соотвествуют заданным, дата создания соотвествует текущему времени</t>
   </si>
 </sst>
 </file>
@@ -1036,6 +1036,7 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -1705,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I50" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1725,7 +1726,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" thickBot="1">
       <c r="A1" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
@@ -1751,7 +1752,7 @@
     </row>
     <row r="2" spans="1:9" ht="56">
       <c r="A2" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>3</v>
@@ -1775,12 +1776,12 @@
         <v>66</v>
       </c>
       <c r="I2" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="140">
       <c r="A3" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B3" s="32"/>
       <c r="C3" s="8" t="s">
@@ -1802,12 +1803,12 @@
         <v>68</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="126">
       <c r="A4" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" s="32"/>
       <c r="C4" s="8" t="s">
@@ -1829,12 +1830,12 @@
         <v>70</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="98">
       <c r="A5" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="8" t="s">
@@ -1856,12 +1857,12 @@
         <v>72</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="112">
       <c r="A6" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="8" t="s">
@@ -1885,7 +1886,7 @@
     </row>
     <row r="7" spans="1:9" ht="112">
       <c r="A7" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="8" t="s">
@@ -1909,7 +1910,7 @@
     </row>
     <row r="8" spans="1:9" ht="126">
       <c r="A8" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="8" t="s">
@@ -1933,7 +1934,7 @@
     </row>
     <row r="9" spans="1:9" ht="84">
       <c r="A9" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="19" t="s">
@@ -1957,7 +1958,7 @@
     </row>
     <row r="10" spans="1:9" ht="84">
       <c r="A10" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="19" t="s">
@@ -1981,7 +1982,7 @@
     </row>
     <row r="11" spans="1:9" ht="140">
       <c r="A11" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="8" t="s">
@@ -2005,7 +2006,7 @@
     </row>
     <row r="12" spans="1:9" ht="140">
       <c r="A12" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="8" t="s">
@@ -2029,7 +2030,7 @@
     </row>
     <row r="13" spans="1:9" ht="140">
       <c r="A13" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B13" s="35"/>
       <c r="C13" s="8" t="s">
@@ -2053,7 +2054,7 @@
     </row>
     <row r="14" spans="1:9" ht="155" customHeight="1" thickBot="1">
       <c r="A14" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="29" t="s">
@@ -2077,7 +2078,7 @@
     </row>
     <row r="15" spans="1:9" ht="168">
       <c r="A15" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>13</v>
@@ -2101,12 +2102,12 @@
         <v>93</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="84">
       <c r="A16" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B16" s="32"/>
       <c r="C16" s="8" t="s">
@@ -2128,12 +2129,12 @@
         <v>96</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="98">
       <c r="A17" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="8" t="s">
@@ -2155,12 +2156,12 @@
         <v>98</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="56">
       <c r="A18" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B18" s="32"/>
       <c r="C18" s="16" t="s">
@@ -2184,7 +2185,7 @@
     </row>
     <row r="19" spans="1:9" ht="28.5" thickBot="1">
       <c r="A19" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="9" t="s">
@@ -2206,12 +2207,12 @@
         <v>104</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="42">
       <c r="A20" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B20" s="31" t="s">
         <v>103</v>
@@ -2235,12 +2236,12 @@
         <v>106</v>
       </c>
       <c r="I20" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="56">
       <c r="A21" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B21" s="32"/>
       <c r="C21" s="8" t="s">
@@ -2262,12 +2263,12 @@
         <v>108</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="42">
       <c r="A22" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B22" s="32"/>
       <c r="C22" s="8" t="s">
@@ -2291,7 +2292,7 @@
     </row>
     <row r="23" spans="1:9" ht="42">
       <c r="A23" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B23" s="32"/>
       <c r="C23" s="8" t="s">
@@ -2315,7 +2316,7 @@
     </row>
     <row r="24" spans="1:9" ht="98">
       <c r="A24" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B24" s="32"/>
       <c r="C24" s="8" t="s">
@@ -2331,18 +2332,18 @@
         <v>115</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="98">
       <c r="A25" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="16" t="s">
@@ -2358,18 +2359,18 @@
         <v>115</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>118</v>
       </c>
       <c r="I25" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="98">
       <c r="A26" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B26" s="32"/>
       <c r="C26" s="8" t="s">
@@ -2385,15 +2386,15 @@
         <v>115</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="112.5" thickBot="1">
       <c r="A27" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="9" t="s">
@@ -2409,18 +2410,18 @@
         <v>119</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="140">
       <c r="A28" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>25</v>
@@ -2444,12 +2445,12 @@
         <v>121</v>
       </c>
       <c r="I28" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="98">
       <c r="A29" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B29" s="32"/>
       <c r="C29" s="8" t="s">
@@ -2471,12 +2472,12 @@
         <v>123</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="56">
       <c r="A30" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="8" t="s">
@@ -2500,7 +2501,7 @@
     </row>
     <row r="31" spans="1:9" ht="70">
       <c r="A31" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B31" s="32"/>
       <c r="C31" s="8" t="s">
@@ -2524,7 +2525,7 @@
     </row>
     <row r="32" spans="1:9" ht="42">
       <c r="A32" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B32" s="32"/>
       <c r="C32" s="8" t="s">
@@ -2548,7 +2549,7 @@
     </row>
     <row r="33" spans="1:9" ht="42">
       <c r="A33" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B33" s="32"/>
       <c r="C33" s="8" t="s">
@@ -2572,7 +2573,7 @@
     </row>
     <row r="34" spans="1:9" ht="140">
       <c r="A34" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B34" s="32"/>
       <c r="C34" s="8" t="s">
@@ -2596,7 +2597,7 @@
     </row>
     <row r="35" spans="1:9" ht="112">
       <c r="A35" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B35" s="32"/>
       <c r="C35" s="8" t="s">
@@ -2620,7 +2621,7 @@
     </row>
     <row r="36" spans="1:9" ht="112">
       <c r="A36" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B36" s="32"/>
       <c r="C36" s="8" t="s">
@@ -2642,12 +2643,12 @@
         <v>137</v>
       </c>
       <c r="I36" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="98">
       <c r="A37" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B37" s="32"/>
       <c r="C37" s="8" t="s">
@@ -2671,7 +2672,7 @@
     </row>
     <row r="38" spans="1:9" ht="112">
       <c r="A38" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B38" s="32"/>
       <c r="C38" s="8" t="s">
@@ -2695,7 +2696,7 @@
     </row>
     <row r="39" spans="1:9" ht="84">
       <c r="A39" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B39" s="32"/>
       <c r="C39" s="8" t="s">
@@ -2717,12 +2718,12 @@
         <v>145</v>
       </c>
       <c r="I39" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="84">
       <c r="A40" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B40" s="32"/>
       <c r="C40" s="8" t="s">
@@ -2744,12 +2745,12 @@
         <v>147</v>
       </c>
       <c r="I40" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="154">
       <c r="A41" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B41" s="32"/>
       <c r="C41" s="8" t="s">
@@ -2771,16 +2772,16 @@
         <v>149</v>
       </c>
       <c r="I41" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="175.5" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B42" s="32"/>
       <c r="C42" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>5</v>
@@ -2789,21 +2790,21 @@
         <v>142</v>
       </c>
       <c r="F42" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="G42" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="G42" s="18" t="s">
+      <c r="H42" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="H42" s="18" t="s">
-        <v>207</v>
-      </c>
       <c r="I42" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="210">
       <c r="A43" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B43" s="32"/>
       <c r="C43" s="16" t="s">
@@ -2816,25 +2817,25 @@
         <v>142</v>
       </c>
       <c r="F43" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="G43" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G43" s="18" t="s">
+      <c r="H43" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="H43" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="I43" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="233.5" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B44" s="32"/>
       <c r="C44" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>9</v>
@@ -2843,18 +2844,18 @@
         <v>142</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G44" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="238">
       <c r="A45" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B45" s="32"/>
       <c r="C45" s="16" t="s">
@@ -2867,22 +2868,22 @@
         <v>142</v>
       </c>
       <c r="F45" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="H45" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="H45" s="18" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="150" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B46" s="35"/>
       <c r="C46" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>9</v>
@@ -2891,18 +2892,18 @@
         <v>142</v>
       </c>
       <c r="F46" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="G46" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="H46" s="18" t="s">
         <v>210</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="140.5" thickBot="1">
       <c r="A47" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B47" s="33"/>
       <c r="C47" s="8" t="s">
@@ -2915,21 +2916,21 @@
         <v>142</v>
       </c>
       <c r="F47" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="G47" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="G47" s="21" t="s">
-        <v>156</v>
-      </c>
       <c r="H47" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="56">
       <c r="A48" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B48" s="31" t="s">
         <v>41</v>
@@ -2941,24 +2942,24 @@
         <v>5</v>
       </c>
       <c r="E48" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F48" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="G48" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="G48" s="15" t="s">
-        <v>159</v>
-      </c>
       <c r="H48" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I48" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="56">
       <c r="A49" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B49" s="32"/>
       <c r="C49" s="8" t="s">
@@ -2968,24 +2969,24 @@
         <v>5</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F49" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G49" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="G49" s="15" t="s">
-        <v>161</v>
-      </c>
       <c r="H49" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I49" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="56.5" thickBot="1">
       <c r="A50" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B50" s="33"/>
       <c r="C50" s="9" t="s">
@@ -2995,21 +2996,21 @@
         <v>9</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F50" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G50" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="H50" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="112">
       <c r="A51" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B51" s="31" t="s">
         <v>44</v>
@@ -3021,24 +3022,24 @@
         <v>5</v>
       </c>
       <c r="E51" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F51" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="G51" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="G51" s="15" t="s">
-        <v>167</v>
-      </c>
       <c r="H51" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I51" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="56">
       <c r="A52" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B52" s="32"/>
       <c r="C52" s="16" t="s">
@@ -3048,24 +3049,24 @@
         <v>9</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F52" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="G52" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="G52" s="18" t="s">
+      <c r="H52" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="H52" s="18" t="s">
-        <v>172</v>
-      </c>
       <c r="I52" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="42.5" thickBot="1">
       <c r="A53" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="22" t="s">
@@ -3075,24 +3076,24 @@
         <v>9</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F53" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="G53" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="G53" s="18" t="s">
-        <v>174</v>
-      </c>
       <c r="H53" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I53" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="98">
       <c r="A54" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B54" s="31" t="s">
         <v>47</v>
@@ -3107,18 +3108,18 @@
         <v>94</v>
       </c>
       <c r="F54" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="G54" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="G54" s="15" t="s">
-        <v>176</v>
-      </c>
       <c r="H54" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="98">
       <c r="A55" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B55" s="32"/>
       <c r="C55" s="8" t="s">
@@ -3131,18 +3132,18 @@
         <v>94</v>
       </c>
       <c r="F55" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="G55" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="G55" s="15" t="s">
-        <v>178</v>
-      </c>
       <c r="H55" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="112">
       <c r="A56" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B56" s="32"/>
       <c r="C56" s="8" t="s">
@@ -3155,18 +3156,18 @@
         <v>94</v>
       </c>
       <c r="F56" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="G56" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="G56" s="15" t="s">
-        <v>180</v>
-      </c>
       <c r="H56" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="98.5" thickBot="1">
       <c r="A57" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B57" s="33"/>
       <c r="C57" s="9" t="s">
@@ -3179,18 +3180,18 @@
         <v>94</v>
       </c>
       <c r="F57" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G57" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="G57" s="15" t="s">
+      <c r="H57" s="15" t="s">
         <v>182</v>
-      </c>
-      <c r="H57" s="15" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="42">
       <c r="A58" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B58" s="31" t="s">
         <v>52</v>
@@ -3205,18 +3206,18 @@
         <v>94</v>
       </c>
       <c r="F58" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="G58" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="G58" s="15" t="s">
-        <v>185</v>
-      </c>
       <c r="H58" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="42">
       <c r="A59" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B59" s="32"/>
       <c r="C59" s="8" t="s">
@@ -3229,18 +3230,18 @@
         <v>94</v>
       </c>
       <c r="F59" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="G59" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="G59" s="15" t="s">
-        <v>187</v>
-      </c>
       <c r="H59" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="42">
       <c r="A60" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B60" s="32"/>
       <c r="C60" s="8" t="s">
@@ -3253,18 +3254,18 @@
         <v>94</v>
       </c>
       <c r="F60" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="G60" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="G60" s="15" t="s">
-        <v>189</v>
-      </c>
       <c r="H60" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="56">
       <c r="A61" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B61" s="32"/>
       <c r="C61" s="8" t="s">
@@ -3277,18 +3278,18 @@
         <v>94</v>
       </c>
       <c r="F61" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="G61" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="G61" s="15" t="s">
-        <v>191</v>
-      </c>
       <c r="H61" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="42">
       <c r="A62" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B62" s="32"/>
       <c r="C62" s="8" t="s">
@@ -3301,18 +3302,18 @@
         <v>94</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="70">
       <c r="A63" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B63" s="32"/>
       <c r="C63" s="8" t="s">
@@ -3325,18 +3326,18 @@
         <v>94</v>
       </c>
       <c r="F63" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="G63" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="G63" s="15" t="s">
-        <v>195</v>
-      </c>
       <c r="H63" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="56">
       <c r="A64" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B64" s="32"/>
       <c r="C64" s="8" t="s">
@@ -3349,18 +3350,18 @@
         <v>94</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="140.5" thickBot="1">
       <c r="A65" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B65" s="33"/>
       <c r="C65" s="22" t="s">
@@ -3373,13 +3374,13 @@
         <v>94</v>
       </c>
       <c r="F65" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G65" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="H65" s="18" t="s">
         <v>199</v>
-      </c>
-      <c r="H65" s="18" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>